<commit_message>
Basic accel value passing
</commit_message>
<xml_diff>
--- a/accel test.xlsx
+++ b/accel test.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$H$44</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="14">
   <si>
     <t>X:</t>
   </si>
@@ -54,6 +58,18 @@
   </si>
   <si>
     <t>Landscape Left Front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count: </t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -373,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -4534,4 +4550,1185 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>-352</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4028</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>856</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>-332</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>4044</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>824</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1294</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3662</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>504</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1610</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>-12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>-3976</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2768</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>786</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1820</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3044</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>198</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>-2924</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>3094</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>-6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1192</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>3334</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>-862</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>-1732</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2296</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>-172</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1990</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>5228</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>-3232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>3196</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1762</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>-1466</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2468</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>-120</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>974</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>3810</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1704</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>-4014</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>4116</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>1052</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>1124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4760</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>-1270</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>-1120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>3200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>3342</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>-1310</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>5480</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>-674</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>-844</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>2174</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>-4346</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>-670</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>2518</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>1624</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>-1224</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>3306</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>790</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>528</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>2816</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>-1540</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>-1644</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>2332</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>1232</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>2062</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>2498</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>-224</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>-1682</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>3856</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>-1002</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>-2076</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>3128</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>2238</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>-2424</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>6114</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>3454</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>3372</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>2028</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>-820</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>-1466</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>3220</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>756</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>-814</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>2064</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>-812</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>5438</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>1260</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>-148</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>-3252</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>4134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>-356</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>-1020</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>2618</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>3996</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>-376</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>2804</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>-1086</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>-544</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>2332</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>-1694</v>
+      </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>-2782</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>2350</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>2448</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>-206</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>7032</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>-1560</v>
+      </c>
+      <c r="G37" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>5080</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>624</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>1642</v>
+      </c>
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>-2196</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>4724</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>-202</v>
+      </c>
+      <c r="G39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>3292</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>4882</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>-90</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>-1204</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>5988</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>710</v>
+      </c>
+      <c r="G41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>832</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>2794</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>-26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>-776</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>2690</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>1650</v>
+      </c>
+      <c r="G43" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>-786</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>3890</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>-1636</v>
+      </c>
+      <c r="G44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H44"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>